<commit_message>
[Edited]: Update function getNewById, findSalakByCid, findSalakBySelf, Add Function GetListRewardAtDate
</commit_message>
<xml_diff>
--- a/data/customer.xlsx
+++ b/data/customer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/BAAC_DATA/@Working_Y63/CodeCampUpSkillBatch1/Project/Group/Final/final-americano-api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20734F8-DA57-3240-A023-7E6143F60AA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59EEB10-4249-CB48-9D5C-8C9D65941C1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" tabRatio="325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerData" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_62" localSheetId="0">CustomerData!#REF!</definedName>
     <definedName name="REPORT6_2" localSheetId="0">CustomerData!#REF!</definedName>
-    <definedName name="REPORT6_3" localSheetId="0">CustomerData!$B$2:$I$11</definedName>
+    <definedName name="REPORT6_3" localSheetId="0">CustomerData!$B$2:$J$11</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="90">
   <si>
     <t>ก็ หน่อทิม</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>90005020</t>
+  </si>
+  <si>
+    <t>BOD</t>
+  </si>
+  <si>
+    <t>1991-09-03</t>
   </si>
 </sst>
 </file>
@@ -348,7 +354,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +383,13 @@
       <color theme="1"/>
       <name val="TH SarabunPSK"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -787,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -798,16 +811,16 @@
     <col min="1" max="1" width="5.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="7.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="31.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="19" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="3"/>
+    <col min="4" max="5" width="24.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="31.1640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="19" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" ht="22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="22" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>68</v>
       </c>
@@ -821,22 +834,25 @@
         <v>71</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -850,23 +866,26 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -880,23 +899,26 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -910,23 +932,26 @@
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -940,23 +965,26 @@
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -970,23 +998,26 @@
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1000,23 +1031,26 @@
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1030,23 +1064,26 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1060,23 +1097,26 @@
         <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1090,23 +1130,26 @@
         <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1120,23 +1163,26 @@
         <v>18</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1150,23 +1196,26 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1180,23 +1229,26 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1210,23 +1262,26 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -1240,26 +1295,30 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:J11">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:K11">
     <sortCondition ref="D1:D11"/>
   </sortState>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[Edited] Add Function MockData and using authen
</commit_message>
<xml_diff>
--- a/data/customer.xlsx
+++ b/data/customer.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/BAAC_DATA/@Working_Y63/CodeCampUpSkillBatch1/Project/Group/Final/final-americano-api/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59EEB10-4249-CB48-9D5C-8C9D65941C1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" tabRatio="325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" tabRatio="325"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerData" sheetId="2" r:id="rId1"/>
@@ -18,15 +12,15 @@
   <definedNames>
     <definedName name="_62" localSheetId="0">CustomerData!#REF!</definedName>
     <definedName name="REPORT6_2" localSheetId="0">CustomerData!#REF!</definedName>
-    <definedName name="REPORT6_3" localSheetId="0">CustomerData!$B$2:$J$11</definedName>
+    <definedName name="REPORT6_3" localSheetId="0">CustomerData!$D$2:$L$11</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="62" type="6" refreshedVersion="4" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="62" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="874" sourceFile="C:\ทีมจัดการข้อมูล\Request\DT_DEPSR0438\62.txt" comma="1">
       <textFields count="9">
         <textField type="text"/>
@@ -41,7 +35,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="REPORT6_2" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="2" name="REPORT6_2" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="874" sourceFile="C:\ทีมจัดการข้อมูล\Request\DT_DEPSR0438\REPORT6_2.txt" comma="1">
       <textFields count="9">
         <textField/>
@@ -56,7 +50,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="REPORT6_21" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="3" name="REPORT6_21" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="874" sourceFile="C:\ทีมจัดการข้อมูล\Request\DT_DEPSR0438\REPORT6_2.txt" comma="1">
       <textFields count="9">
         <textField type="text"/>
@@ -77,66 +71,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="90">
   <si>
-    <t>ก็ หน่อทิม</t>
-  </si>
-  <si>
-    <t xml:space="preserve">นางสาว ก็ หน่อทิม   </t>
-  </si>
-  <si>
-    <t>กช ภูหมั่นเพียร</t>
-  </si>
-  <si>
-    <t xml:space="preserve">นางสาว กช ภูหมั่นเพียร   </t>
-  </si>
-  <si>
-    <t>กชกนก แสงสิทธิ์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">น.ส. กชกนก แสงสิทธิ์   </t>
-  </si>
-  <si>
-    <t>กชกมล กมลสุวรรณ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">นางสาว กชกมล กมลสุวรรณ   </t>
-  </si>
-  <si>
-    <t>กชกมล ภูชิตจตุรภัทร์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">นางสาว กชกมล ภูชิตจตุรภัทร์   </t>
-  </si>
-  <si>
-    <t>กชกร กอบคำ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">นางสาว กชกร กอบคำ   </t>
-  </si>
-  <si>
-    <t>กชกร จารุเรืองสุข</t>
-  </si>
-  <si>
-    <t xml:space="preserve">นางสาว กชกร จารุเรืองสุข   </t>
-  </si>
-  <si>
-    <t>กชกร ชัยเชิดชู</t>
-  </si>
-  <si>
-    <t xml:space="preserve">นางสาว กชกร ชัยเชิดชู   </t>
-  </si>
-  <si>
-    <t>กชกร ดุลยพัชร์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">นางสาว กชกร ดุลยพัชร์   </t>
-  </si>
-  <si>
-    <t>กชกร นันทะวงศ์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">นางสาว กชกร นันทะวงศ์   </t>
-  </si>
-  <si>
     <t>80000000</t>
   </si>
   <si>
@@ -345,20 +279,80 @@
   </si>
   <si>
     <t>1991-09-03</t>
+  </si>
+  <si>
+    <t>กชใจ เพียร</t>
+  </si>
+  <si>
+    <t xml:space="preserve">นางสาว กชใจ เพียร </t>
+  </si>
+  <si>
+    <t xml:space="preserve">น.ส. นก แสง  </t>
+  </si>
+  <si>
+    <t>นก แสง</t>
+  </si>
+  <si>
+    <t>นางสาว ก็ได้ หน่อทิมมาน</t>
+  </si>
+  <si>
+    <t>ก็ได้ หน่อทิมมาน</t>
+  </si>
+  <si>
+    <t>กมล สุวรรณ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">นางสาว กมล สุวรรณ  </t>
+  </si>
+  <si>
+    <t>แสง ภูชิต</t>
+  </si>
+  <si>
+    <t xml:space="preserve">นางสาว แสง ภูชิต </t>
+  </si>
+  <si>
+    <t>กี กอบ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">นางสาว กี กอบ </t>
+  </si>
+  <si>
+    <t>สี สุข</t>
+  </si>
+  <si>
+    <t xml:space="preserve">นางสาว สี สุข </t>
+  </si>
+  <si>
+    <t>ชู ชัย</t>
+  </si>
+  <si>
+    <t>กร พัชร์</t>
+  </si>
+  <si>
+    <t>นางสาว กร พัชร์</t>
+  </si>
+  <si>
+    <t>นัน วงศ์</t>
+  </si>
+  <si>
+    <t xml:space="preserve">นางสาว นัน วงศ์   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">นางสาว ชู ชัย   </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -366,7 +360,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -386,7 +380,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -426,7 +420,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -476,7 +470,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="REPORT6_3" connectionId="3" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="REPORT6_3" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -522,7 +516,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -555,26 +549,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -607,23 +584,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -799,524 +759,541 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E8" activeCellId="1" sqref="A7:D8 E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="5" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="4" customWidth="1"/>
-    <col min="4" max="5" width="24.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="31.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="31.125" style="3" customWidth="1"/>
     <col min="9" max="9" width="19" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>63</v>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>51</v>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>52</v>
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>48</v>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>49</v>
+        <v>27</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>45</v>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>57</v>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>58</v>
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>60</v>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>61</v>
+        <v>39</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>39</v>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>40</v>
+        <v>18</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>42</v>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>66</v>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>67</v>
+        <v>45</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>54</v>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>55</v>
+        <v>33</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>63</v>
+      <c r="B12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="I12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>63</v>
+      <c r="B13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="I13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>80</v>
+        <v>42</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>63</v>
+      <c r="B15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>80</v>
+        <v>42</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K15" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:K11">
-    <sortCondition ref="D1:D11"/>
+  <sortState ref="D1:M11">
+    <sortCondition ref="E1:E11"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Edited] Update Mock Customer
</commit_message>
<xml_diff>
--- a/data/customer.xlsx
+++ b/data/customer.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955B7274-1B81-EF4A-B8F7-4BEACD62A72C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" tabRatio="325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerData" sheetId="2" r:id="rId1"/>
@@ -12,15 +18,15 @@
   <definedNames>
     <definedName name="_62" localSheetId="0">CustomerData!#REF!</definedName>
     <definedName name="REPORT6_2" localSheetId="0">CustomerData!#REF!</definedName>
-    <definedName name="REPORT6_3" localSheetId="0">CustomerData!$D$2:$L$11</definedName>
+    <definedName name="REPORT6_3" localSheetId="0">CustomerData!$D$2:$J$11</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="62" type="6" refreshedVersion="4" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="62" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="874" sourceFile="C:\ทีมจัดการข้อมูล\Request\DT_DEPSR0438\62.txt" comma="1">
       <textFields count="9">
         <textField type="text"/>
@@ -35,7 +41,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="REPORT6_2" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="REPORT6_2" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="874" sourceFile="C:\ทีมจัดการข้อมูล\Request\DT_DEPSR0438\REPORT6_2.txt" comma="1">
       <textFields count="9">
         <textField/>
@@ -50,7 +56,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="REPORT6_21" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="REPORT6_21" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="874" sourceFile="C:\ทีมจัดการข้อมูล\Request\DT_DEPSR0438\REPORT6_2.txt" comma="1">
       <textFields count="9">
         <textField type="text"/>
@@ -69,61 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="90">
-  <si>
-    <t>80000000</t>
-  </si>
-  <si>
-    <t>80000199</t>
-  </si>
-  <si>
-    <t>80000200</t>
-  </si>
-  <si>
-    <t>80000202</t>
-  </si>
-  <si>
-    <t>80000203</t>
-  </si>
-  <si>
-    <t>80000222</t>
-  </si>
-  <si>
-    <t>80000223</t>
-  </si>
-  <si>
-    <t>80000622</t>
-  </si>
-  <si>
-    <t>80000623</t>
-  </si>
-  <si>
-    <t>80000642</t>
-  </si>
-  <si>
-    <t>80000643</t>
-  </si>
-  <si>
-    <t>80000644</t>
-  </si>
-  <si>
-    <t>80000645</t>
-  </si>
-  <si>
-    <t>80000744</t>
-  </si>
-  <si>
-    <t>80000745</t>
-  </si>
-  <si>
-    <t>80000794</t>
-  </si>
-  <si>
-    <t>80000795</t>
-  </si>
-  <si>
-    <t>80000894</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="101">
   <si>
     <t>1100800964478</t>
   </si>
@@ -239,42 +191,12 @@
     <t>SalakEnd</t>
   </si>
   <si>
-    <t>80002000</t>
-  </si>
-  <si>
-    <t>80002010</t>
-  </si>
-  <si>
-    <t>80003000</t>
-  </si>
-  <si>
-    <t>80003020</t>
-  </si>
-  <si>
     <t>500031732945</t>
   </si>
   <si>
-    <t>90004000</t>
-  </si>
-  <si>
-    <t>90004020</t>
-  </si>
-  <si>
     <t>AccType</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>90005000</t>
-  </si>
-  <si>
-    <t>90005020</t>
-  </si>
-  <si>
     <t>BOD</t>
   </si>
   <si>
@@ -339,20 +261,137 @@
   </si>
   <si>
     <t xml:space="preserve">นางสาว ชู ชัย   </t>
+  </si>
+  <si>
+    <t>9182400</t>
+  </si>
+  <si>
+    <t>9182300</t>
+  </si>
+  <si>
+    <t>5040800</t>
+  </si>
+  <si>
+    <t>5040900</t>
+  </si>
+  <si>
+    <t>5680600</t>
+  </si>
+  <si>
+    <t>5680700</t>
+  </si>
+  <si>
+    <t>7512500</t>
+  </si>
+  <si>
+    <t>7512600</t>
+  </si>
+  <si>
+    <t>2851300</t>
+  </si>
+  <si>
+    <t>2851400</t>
+  </si>
+  <si>
+    <t>4041100</t>
+  </si>
+  <si>
+    <t>4041150</t>
+  </si>
+  <si>
+    <t>9949600</t>
+  </si>
+  <si>
+    <t>9949700</t>
+  </si>
+  <si>
+    <t>8000223</t>
+  </si>
+  <si>
+    <t>8000622</t>
+  </si>
+  <si>
+    <t>8000623</t>
+  </si>
+  <si>
+    <t>8000642</t>
+  </si>
+  <si>
+    <t>8000643</t>
+  </si>
+  <si>
+    <t>8000644</t>
+  </si>
+  <si>
+    <t>8000645</t>
+  </si>
+  <si>
+    <t>8000744</t>
+  </si>
+  <si>
+    <t>8000745</t>
+  </si>
+  <si>
+    <t>8000794</t>
+  </si>
+  <si>
+    <t>8000795</t>
+  </si>
+  <si>
+    <t>8000894</t>
+  </si>
+  <si>
+    <t>8038500</t>
+  </si>
+  <si>
+    <t>8038400</t>
+  </si>
+  <si>
+    <t>8038510</t>
+  </si>
+  <si>
+    <t>8038780</t>
+  </si>
+  <si>
+    <t>4609300</t>
+  </si>
+  <si>
+    <t>4609400</t>
+  </si>
+  <si>
+    <t>9488700</t>
+  </si>
+  <si>
+    <t>9488800</t>
+  </si>
+  <si>
+    <t>6358700</t>
+  </si>
+  <si>
+    <t>6358800</t>
+  </si>
+  <si>
+    <t>สลาก ธ.ก.ส.ชุดเกษตรมั่งคั่ง 2</t>
+  </si>
+  <si>
+    <t>สลาก ธ.ก.ส.ชุดเกษตรมั่งคั่ง 3</t>
+  </si>
+  <si>
+    <t>สลาก ธ.ก.ส.ชุดเกษตรมั่งคั่ง 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -360,7 +399,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -380,7 +419,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -420,7 +459,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -470,7 +509,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="REPORT6_3" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="REPORT6_3" connectionId="3" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -516,7 +555,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -549,9 +588,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,6 +640,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -759,540 +832,670 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E8" activeCellId="1" sqref="A7:D8 E8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="24.125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="7.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="31.125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="31.1640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="19" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="3"/>
+    <col min="10" max="10" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="44" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="11">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="11">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="11">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="1" t="s">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="11">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+      <c r="F19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="11">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="D1:M11">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:K11">
     <sortCondition ref="E1:E11"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>